<commit_message>
Removed .env file from tracking
</commit_message>
<xml_diff>
--- a/rest_format.xlsx
+++ b/rest_format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\projects\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BFCCEF-8CE2-4621-A6AB-D7BF9F884D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F2C683-0AA7-4049-A34C-4C2B437CD4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15FD23A8-80B3-44FC-AEB5-CBEFF97BBD21}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>api_end_point</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:8000/chat/&lt;chatroom_name&gt;/</t>
   </si>
   <si>
     <t>json format</t>
@@ -224,12 +221,21 @@
 "roles":"admin,user"
 }</t>
   </si>
+  <si>
+    <t>ws://127.0.0.1:8000/ws/chat/problem1434/</t>
+  </si>
+  <si>
+    <t>{"room":"room3"}</t>
+  </si>
+  <si>
+    <t>addition of rooms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +250,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -267,12 +285,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -590,13 +610,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3332A2-9346-474B-A2C1-DE512B9D8F97}">
   <dimension ref="C4:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" customWidth="1"/>
     <col min="8" max="8" width="39.88671875" customWidth="1"/>
@@ -607,114 +627,124 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
-        <v>4</v>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="3:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" t="s">
         <v>7</v>
-      </c>
-      <c r="I11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="201.6" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="35" spans="3:8" ht="374.4" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
         <v>12</v>
       </c>
-      <c r="E35" t="s">
+      <c r="H35" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="39" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="3:8" ht="72" x14ac:dyDescent="0.3">
       <c r="H40" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
         <v>18</v>
       </c>
-      <c r="E45" t="s">
+      <c r="H45" t="s">
         <v>19</v>
-      </c>
-      <c r="H45" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="49" spans="3:8" ht="72" x14ac:dyDescent="0.3">
       <c r="C49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E49" t="s">
-        <v>23</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="55" spans="3:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" t="s">
         <v>24</v>
       </c>
-      <c r="E55" t="s">
+      <c r="H55" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{C2B5051A-AEDF-43D3-823A-C9EED0060BA2}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{CE1F6612-83EC-4C8D-91EC-CCE7A06CB067}"/>
-    <hyperlink ref="C23" r:id="rId3" xr:uid="{5C5835CC-AF86-45A2-9A35-F8D6F2A6776A}"/>
-    <hyperlink ref="C35" r:id="rId4" xr:uid="{BF73B8B9-B902-497F-A71B-F98AFDD78E65}"/>
-    <hyperlink ref="C39" r:id="rId5" xr:uid="{E87575F5-6491-4093-9360-55264B0C88FC}"/>
-    <hyperlink ref="C45" r:id="rId6" xr:uid="{3362D68B-9822-41CE-B34A-E2DCEDDE4194}"/>
-    <hyperlink ref="C49" r:id="rId7" xr:uid="{164DC237-375E-495D-A630-1AA9DF93A9F2}"/>
-    <hyperlink ref="C55" r:id="rId8" xr:uid="{CB26DAC7-0B0F-4A04-979A-28125718E366}"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{CE1F6612-83EC-4C8D-91EC-CCE7A06CB067}"/>
+    <hyperlink ref="C23" r:id="rId2" xr:uid="{5C5835CC-AF86-45A2-9A35-F8D6F2A6776A}"/>
+    <hyperlink ref="C35" r:id="rId3" xr:uid="{BF73B8B9-B902-497F-A71B-F98AFDD78E65}"/>
+    <hyperlink ref="C39" r:id="rId4" xr:uid="{E87575F5-6491-4093-9360-55264B0C88FC}"/>
+    <hyperlink ref="C45" r:id="rId5" xr:uid="{3362D68B-9822-41CE-B34A-E2DCEDDE4194}"/>
+    <hyperlink ref="C49" r:id="rId6" xr:uid="{164DC237-375E-495D-A630-1AA9DF93A9F2}"/>
+    <hyperlink ref="C55" r:id="rId7" xr:uid="{CB26DAC7-0B0F-4A04-979A-28125718E366}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>